<commit_message>
Assert Libary updated with more assertion
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestInput.xlsx
+++ b/src/test/resources/excel/TestInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksh\git\ataf\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F01FFB0-9AE3-4BB9-9213-95A012E7C75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF99A01-728E-4A05-8811-31212A22872A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{95E5B64E-F434-4F35-8E70-B90CC0CDD42B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{95E5B64E-F434-4F35-8E70-B90CC0CDD42B}"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Yes</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>Ignore Value List</t>
+  </si>
+  <si>
+    <t>JsonPath</t>
+  </si>
+  <si>
+    <t>$.title</t>
+  </si>
+  <si>
+    <t>BMW Pencil</t>
+  </si>
+  <si>
+    <t>Expected Value</t>
   </si>
   <si>
     <t>images</t>
@@ -507,17 +519,17 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -531,7 +543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -545,7 +557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -559,7 +571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -580,22 +592,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9E4029-3958-4C69-854D-2D54083BF57F}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="A1:G4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -617,8 +631,14 @@
       <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="H1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -640,8 +660,14 @@
       <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
@@ -663,8 +689,14 @@
       <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -679,9 +711,15 @@
         <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>